<commit_message>
done with metadata import
</commit_message>
<xml_diff>
--- a/example/metadata/FAANG/FAANG_GGA_UD_1004&1014.xlsx
+++ b/example/metadata/FAANG/FAANG_GGA_UD_1004&1014.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/modupe/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/modupe/TAD/example/metadata/FAANG/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="24640" windowHeight="14180" tabRatio="612"/>
+    <workbookView xWindow="-23080" yWindow="1040" windowWidth="24640" windowHeight="14180" tabRatio="612" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="131">
   <si>
     <t>NCBI Taxonomy</t>
   </si>
@@ -267,9 +267,6 @@
     <t>availability</t>
   </si>
   <si>
-    <t>tissue</t>
-  </si>
-  <si>
     <t>specimen collection protocol</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>UBERON_0000007</t>
   </si>
   <si>
-    <t>GGA_UD_1004Pit</t>
-  </si>
-  <si>
     <t>tissue specimen</t>
   </si>
   <si>
@@ -435,7 +429,7 @@
     <t>grams</t>
   </si>
   <si>
-    <t>GGA_UD_1014Pit</t>
+    <t>organism part</t>
   </si>
 </sst>
 </file>
@@ -1733,7 +1727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1836,13 +1830,13 @@
         <v>75</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>5</v>
@@ -2332,7 +2326,7 @@
         <v>75</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>5</v>
@@ -2341,7 +2335,7 @@
         <v>6</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>5</v>
@@ -2350,13 +2344,13 @@
         <v>6</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2824,10 +2818,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2872,19 +2866,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="E2" t="s">
         <v>101</v>
-      </c>
-      <c r="E2" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2927,16 +2921,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>105</v>
-      </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3130,8 +3124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3295,61 +3289,61 @@
     </row>
     <row r="2" spans="1:38" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>106</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>107</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="8"/>
       <c r="M2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>26</v>
       </c>
       <c r="R2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="S2" s="13" t="s">
         <v>115</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>116</v>
       </c>
       <c r="T2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V2" s="33"/>
       <c r="W2" s="34"/>
@@ -3371,61 +3365,61 @@
     </row>
     <row r="3" spans="1:38" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>106</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>107</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="8"/>
       <c r="M3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O3" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="P3" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="Q3" s="13" t="s">
         <v>26</v>
       </c>
       <c r="R3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="S3" s="13" t="s">
         <v>115</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>116</v>
       </c>
       <c r="T3" s="13" t="s">
         <v>15</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V3" s="33"/>
       <c r="W3" s="34"/>
@@ -4903,7 +4897,7 @@
   <dimension ref="A1:AG165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4970,7 +4964,7 @@
         <v>75</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>5</v>
@@ -4979,22 +4973,22 @@
         <v>6</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="37" t="s">
         <v>77</v>
-      </c>
-      <c r="M1" s="37" t="s">
-        <v>78</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>5</v>
@@ -5003,7 +4997,7 @@
         <v>6</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>5</v>
@@ -5012,34 +5006,34 @@
         <v>6</v>
       </c>
       <c r="W1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="Z1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="AC1" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AD1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="AE1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF1" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="AG1" s="7" t="s">
         <v>9</v>
@@ -5047,147 +5041,147 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L2" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="M2" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="O2" s="13">
         <v>21</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="T2" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC2" s="12">
         <v>0.01</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AG2" s="30"/>
     </row>
     <row r="3" spans="1:33" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L3" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="M3" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="O3" s="13">
         <v>21</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U3" s="13" t="s">
         <v>15</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC3" s="12">
         <v>0.01</v>
       </c>
       <c r="AD3" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="17" x14ac:dyDescent="0.2">

</xml_diff>